<commit_message>
Final push for Ass 3
</commit_message>
<xml_diff>
--- a/Python/Assignment3/CalibratE.xlsx
+++ b/Python/Assignment3/CalibratE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stellenbosch-my.sharepoint.com/personal/21642818_sun_ac_za/Documents/3rd Year EE/E Design 344/E344/Python/Assignment3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="311" documentId="8_{DA5A3A63-BFF6-44F1-9A77-C33E9A7AD195}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D4D2C5E5-9D4B-4EFE-B883-93DFABBB53B5}"/>
+  <xr:revisionPtr revIDLastSave="371" documentId="8_{DA5A3A63-BFF6-44F1-9A77-C33E9A7AD195}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CA46F1D3-AE11-4DFD-80A6-5BAA0EDAD82C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,9 +17,9 @@
   </sheets>
   <definedNames>
     <definedName name="alpha">Sheet1!$B$7</definedName>
-    <definedName name="CONST">Sheet1!$H$28</definedName>
+    <definedName name="CONST">Sheet1!$I$28</definedName>
     <definedName name="gain">Sheet1!$B$8</definedName>
-    <definedName name="M">Sheet1!$G$28</definedName>
+    <definedName name="M">Sheet1!$H$28</definedName>
     <definedName name="vgnd">Sheet1!$B$4</definedName>
     <definedName name="voffset">Sheet1!$B$5</definedName>
     <definedName name="vso">Sheet1!$B$6</definedName>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Temperature Calibration</t>
   </si>
@@ -160,13 +160,17 @@
   <si>
     <t>BPM Calibrated</t>
   </si>
+  <si>
+    <t>Vout_analytical</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="171" formatCode="0.0000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -220,13 +224,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -236,6 +243,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,7 +480,7 @@
             <c:numRef>
               <c:f>Sheet1!$D$27:$D$37</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>51.3347022587269</c:v>
@@ -735,6 +743,17 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vsense</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -829,6 +848,17 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vout</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -879,7 +909,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$12:$E$20</c:f>
+              <c:f>Sheet1!$F$12:$F$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -917,6 +947,75 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-B899-4EF2-BD5D-021DF88F4274}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vout_analytical</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$12:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.6000000000000032</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0000000000000036</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.7999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.6000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.0000000000000009</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.4000000000000012</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.8000000000000016</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-CFCE-42BA-A520-F5DBE7E606EF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2221,13 +2320,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>33337</xdr:rowOff>
@@ -2257,13 +2356,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>461962</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>100012</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>157162</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>176212</xdr:rowOff>
@@ -2557,62 +2656,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:I37"/>
+  <dimension ref="A2:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="18.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="4" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="6"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="5">
-        <f>0.477</f>
-        <v>0.47699999999999998</v>
+        <f>2.2</f>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="F4" s="7" t="s">
+      <c r="G4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="5">
-        <v>1.28</v>
+        <v>1.38</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5">
-        <f>E20-E12</f>
+      <c r="H5" s="2"/>
+      <c r="I5">
+        <f>F20-F12</f>
         <v>3.657188474978986</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -2620,18 +2720,18 @@
         <v>0.62</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>21</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <f>C20-C12</f>
         <v>8</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -2639,37 +2739,38 @@
         <v>0.02</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>22</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <f>POWER(2,10)</f>
         <v>1024</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="5">
+        <f>20</f>
         <v>20</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>23</v>
       </c>
-      <c r="H8">
-        <f>H5*1000/H7</f>
+      <c r="I8">
+        <f>I5*1000/I7</f>
         <v>3.5714731200966661</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
@@ -2677,160 +2778,294 @@
         <f>alpha*38+vso</f>
         <v>1.38</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>24</v>
       </c>
-      <c r="H9">
-        <f>H6/H7</f>
+      <c r="I9">
+        <f>I6/I7</f>
         <v>7.8125E-3</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="J9" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="C11" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="4"/>
+      <c r="F11" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f>FLOOR((B12*POWER(2,10)/5),1)</f>
+        <v>122</v>
+      </c>
+      <c r="B12">
+        <f>gain*(D12-voffset)+vgnd</f>
+        <v>0.6000000000000032</v>
+      </c>
       <c r="C12">
         <v>34</v>
       </c>
       <c r="D12">
-        <f t="shared" ref="D12:D20" si="0">alpha*C12+vso</f>
+        <f>alpha*C12+vso</f>
         <v>1.3</v>
       </c>
       <c r="E12">
+        <f>FLOOR((F12*POWER(2,10)/5),1)</f>
+        <v>40</v>
+      </c>
+      <c r="F12">
         <v>0.19708341375392399</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" ref="A13:A20" si="0">FLOOR((B13*POWER(2,10)/5),1)</f>
+        <v>204</v>
+      </c>
+      <c r="B13">
+        <f t="shared" ref="B13:B20" si="1">gain*(D13-voffset)+vgnd</f>
+        <v>1.0000000000000036</v>
+      </c>
       <c r="C13">
         <v>35</v>
       </c>
       <c r="D13">
+        <f t="shared" ref="D13:D20" si="2">alpha*C13+vso</f>
+        <v>1.32</v>
+      </c>
+      <c r="E13">
+        <f t="shared" ref="E13:E20" si="3">FLOOR((F13*POWER(2,10)/5),1)</f>
+        <v>133</v>
+      </c>
+      <c r="F13">
+        <v>0.65423196615385204</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
         <f t="shared" si="0"/>
-        <v>1.32</v>
-      </c>
-      <c r="E13">
-        <v>0.65423196615385204</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>286</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="1"/>
+        <v>1.3999999999999995</v>
+      </c>
       <c r="C14">
         <v>36</v>
       </c>
       <c r="D14">
+        <f t="shared" si="2"/>
+        <v>1.3399999999999999</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="3"/>
+        <v>227</v>
+      </c>
+      <c r="F14">
+        <v>1.1113789875304401</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" s="9"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
         <f t="shared" si="0"/>
-        <v>1.3399999999999999</v>
-      </c>
-      <c r="E14">
-        <v>1.1113789875304401</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H14" s="8"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>368</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="1"/>
+        <v>1.7999999999999998</v>
+      </c>
       <c r="C15">
         <v>37</v>
       </c>
       <c r="D15">
+        <f t="shared" si="2"/>
+        <v>1.3599999999999999</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="3"/>
+        <v>321</v>
+      </c>
+      <c r="F15">
+        <v>1.5685279369354199</v>
+      </c>
+      <c r="H15" cm="1">
+        <f t="array" ref="H15:I15">LINEST(C12:C20,B12:B20,TRUE,)</f>
+        <v>2.5000000000000004</v>
+      </c>
+      <c r="I15">
+        <v>32.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
         <f t="shared" si="0"/>
-        <v>1.3599999999999999</v>
-      </c>
-      <c r="E15">
-        <v>1.5685279369354199</v>
-      </c>
-      <c r="G15" cm="1">
-        <f t="array" ref="G15:H15">LINEST(C12:C20,E12:E20,TRUE,FALSE)</f>
-        <v>2.1874728435052844</v>
-      </c>
-      <c r="H15">
-        <v>33.56888665728389</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>450</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="1"/>
+        <v>2.2000000000000002</v>
+      </c>
       <c r="C16">
         <v>38</v>
       </c>
       <c r="D16">
+        <f t="shared" si="2"/>
+        <v>1.38</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="3"/>
+        <v>414</v>
+      </c>
+      <c r="F16">
+        <v>2.0256764888763401</v>
+      </c>
+      <c r="H16" cm="1">
+        <f t="array" ref="H16:I16">LINEST(C12:C20,F12:F20,TRUE,FALSE)</f>
+        <v>2.1874728435052844</v>
+      </c>
+      <c r="I16">
+        <v>33.56888665728389</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17">
         <f t="shared" si="0"/>
-        <v>1.38</v>
-      </c>
-      <c r="E16">
-        <v>2.0256764888763401</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+        <v>532</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="1"/>
+        <v>2.6000000000000005</v>
+      </c>
       <c r="C17">
         <v>39</v>
       </c>
       <c r="D17">
+        <f t="shared" si="2"/>
+        <v>1.4</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="3"/>
+        <v>508</v>
+      </c>
+      <c r="F17">
+        <v>2.48282623291015</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18">
         <f t="shared" si="0"/>
-        <v>1.4</v>
-      </c>
-      <c r="E17">
-        <v>2.48282623291015</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+        <v>614</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="1"/>
+        <v>3.0000000000000009</v>
+      </c>
       <c r="C18">
         <v>40</v>
       </c>
       <c r="D18">
+        <f t="shared" si="2"/>
+        <v>1.42</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="3"/>
+        <v>602</v>
+      </c>
+      <c r="F18">
+        <v>2.9399735927581698</v>
+      </c>
+      <c r="H18" cm="1">
+        <f t="array" ref="H18:I18">LINEST(C12:C20,A12:A20,TRUE,FALSE)</f>
+        <v>1.2195121951219514E-2</v>
+      </c>
+      <c r="I18">
+        <v>32.512195121951216</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19">
         <f t="shared" si="0"/>
-        <v>1.42</v>
-      </c>
-      <c r="E18">
-        <v>2.9399735927581698</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+        <v>696</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="1"/>
+        <v>3.4000000000000012</v>
+      </c>
       <c r="C19">
         <v>41</v>
       </c>
       <c r="D19">
+        <f t="shared" si="2"/>
+        <v>1.44</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="3"/>
+        <v>695</v>
+      </c>
+      <c r="F19">
+        <v>3.39712214469909</v>
+      </c>
+      <c r="H19" cm="1">
+        <f t="array" ref="H19:I19">LINEST(C12:C20,E12:E20,TRUE,FALSE)</f>
+        <v>1.0678043403899511E-2</v>
+      </c>
+      <c r="I19">
+        <v>33.5757306829843</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20">
         <f t="shared" si="0"/>
-        <v>1.44</v>
-      </c>
-      <c r="E19">
-        <v>3.39712214469909</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+        <v>778</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="1"/>
+        <v>3.8000000000000016</v>
+      </c>
       <c r="C20">
         <v>42</v>
       </c>
       <c r="D20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.46</v>
       </c>
       <c r="E20">
+        <f t="shared" si="3"/>
+        <v>789</v>
+      </c>
+      <c r="F20">
         <v>3.8542718887329102</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="7" t="s">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="6"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
         <v>10</v>
       </c>
@@ -2840,241 +3075,242 @@
       <c r="D26" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="4"/>
+      <c r="F26" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G26" s="7" t="s">
+      <c r="H26" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>50</v>
       </c>
       <c r="C27">
         <v>55.452865064694997</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="10">
         <v>51.3347022587269</v>
       </c>
-      <c r="E27">
-        <f>(M*D27)+CONST</f>
+      <c r="F27">
+        <f t="shared" ref="F27:F37" si="4">(M*D27)+CONST</f>
         <v>50.331359470635469</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="H27" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H27" s="6"/>
+      <c r="I27" s="7"/>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>60</v>
       </c>
       <c r="C28">
         <v>62.532569046378299</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="10">
         <v>60.749240634491997</v>
       </c>
-      <c r="E28">
-        <f>(M*D28)+CONST</f>
+      <c r="F28">
+        <f t="shared" si="4"/>
         <v>59.903192060769172</v>
       </c>
-      <c r="G28" cm="1">
-        <f t="array" ref="G28:H28">LINEST(B27:B37,D27:D37,TRUE,FALSE)</f>
+      <c r="H28" cm="1">
+        <f t="array" ref="H28:I28">LINEST(B27:B37,D27:D37,TRUE,FALSE)</f>
         <v>1.0167075865104034</v>
       </c>
-      <c r="H28">
+      <c r="I28">
         <v>-1.8610217670649121</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>70</v>
       </c>
       <c r="C29">
         <v>71.428571428571402</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="10">
         <v>70.754716981132006</v>
       </c>
-      <c r="E29">
-        <f>(M*D29)+CONST</f>
+      <c r="F29">
+        <f t="shared" si="4"/>
         <v>70.075835769048467</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>80</v>
       </c>
       <c r="C30">
         <v>82.023239917976696</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="10">
         <v>80.567811241127899</v>
       </c>
-      <c r="E30">
-        <f>(M*D30)+CONST</f>
+      <c r="F30">
+        <f t="shared" si="4"/>
         <v>80.052883150327986</v>
       </c>
-      <c r="G30" s="7" t="s">
+      <c r="H30" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>90</v>
       </c>
       <c r="C31">
         <v>89.485458612975293</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="10">
         <v>90.073184462375593</v>
       </c>
-      <c r="E31">
-        <f>(M*D31)+CONST</f>
+      <c r="F31">
+        <f t="shared" si="4"/>
         <v>89.71706821698335</v>
       </c>
-      <c r="G31" s="6" t="s">
+      <c r="H31" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>100</v>
       </c>
       <c r="C32">
         <v>99.557522123893804</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="10">
         <v>99.889012208656993</v>
       </c>
-      <c r="E32">
-        <f>(M*D32)+CONST</f>
+      <c r="F32">
+        <f t="shared" si="4"/>
         <v>99.696894754506957</v>
       </c>
-      <c r="G32" cm="1">
-        <f t="array" ref="G32:H32">LINEST(B27:B37,LN(C27:C37),TRUE,FALSE)</f>
+      <c r="H32" cm="1">
+        <f t="array" ref="H32:I32">LINEST(B27:B37,LN(C27:C37),TRUE,FALSE)</f>
         <v>99.573393999906429</v>
       </c>
-      <c r="H32">
+      <c r="I32">
         <v>-354.5555182811716</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>110</v>
       </c>
       <c r="C33">
         <v>109.09090909090899</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="10">
         <v>109.70927043335099</v>
       </c>
-      <c r="E33">
-        <f>(M*D33)+CONST</f>
+      <c r="F33">
+        <f t="shared" si="4"/>
         <v>109.68122579304453</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>120</v>
       </c>
       <c r="C34">
         <v>120.643431635388</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="10">
         <v>120.174799708667</v>
       </c>
-      <c r="E34">
-        <f>(M*D34)+CONST</f>
+      <c r="F34">
+        <f t="shared" si="4"/>
         <v>120.32160880410504</v>
       </c>
-      <c r="G34" s="7" t="s">
+      <c r="H34" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>130</v>
       </c>
       <c r="C35">
         <v>129.65964343598</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="10">
         <v>129.70635921455499</v>
       </c>
-      <c r="E35">
-        <f>(M*D35)+CONST</f>
+      <c r="F35">
+        <f t="shared" si="4"/>
         <v>130.0124176650167</v>
       </c>
-      <c r="G35" s="6" t="s">
+      <c r="H35" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>140</v>
       </c>
       <c r="C36">
         <v>140.18691588785001</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="10">
         <v>139.65980304386699</v>
       </c>
-      <c r="E36">
-        <f>(M*D36)+CONST</f>
+      <c r="F36">
+        <f t="shared" si="4"/>
         <v>140.13215951818336</v>
       </c>
-      <c r="G36" cm="1">
-        <f t="array" ref="G36:I36">LINEST(B27:B37,C27:C37^{1,2},TRUE,FALSE)</f>
+      <c r="H36" cm="1">
+        <f t="array" ref="H36:J36">LINEST(B27:B37,C27:C37^{1,2},TRUE,FALSE)</f>
         <v>-1.0293313143591167E-3</v>
       </c>
-      <c r="H36">
+      <c r="I36">
         <v>1.2581610621435411</v>
       </c>
-      <c r="I36">
+      <c r="J36">
         <v>-15.407847973961244</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>150</v>
       </c>
       <c r="C37">
         <v>148.514851485148</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="10">
         <v>149.43960149439599</v>
       </c>
-      <c r="E37">
-        <f>(M*D37)+CONST</f>
+      <c r="F37">
+        <f t="shared" si="4"/>
         <v>150.07535479737891</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="G34:I34"/>
-    <mergeCell ref="G35:I35"/>
+    <mergeCell ref="H31:J31"/>
+    <mergeCell ref="H34:J34"/>
+    <mergeCell ref="H35:J35"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B24:D24"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="H26:J26"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H30:J30"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="H14:I14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>